<commit_message>
mostly finished cleaning data and begun on integrating bin pack
</commit_message>
<xml_diff>
--- a/data_test.xlsx
+++ b/data_test.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mealt\Documents\GitHub\IE-431-Senior-Design-Telamon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E853E60A-A1F7-43D9-8A0F-093B9137933F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422443EE-3255-4692-B986-2A5AB8A573B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="shipping_data_test" sheetId="1" r:id="rId1"/>
-    <sheet name="product_data_test" sheetId="2" r:id="rId2"/>
+    <sheet name="Bins" sheetId="3" r:id="rId1"/>
+    <sheet name="Items" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,21 +26,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
-  <si>
-    <t>Product ID</t>
-  </si>
-  <si>
-    <t>Shipping Order Num</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>W</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Bin Name</t>
+  </si>
+  <si>
+    <t>Bin 1</t>
+  </si>
+  <si>
+    <t>Bin 2</t>
+  </si>
+  <si>
+    <t>Item Name</t>
+  </si>
+  <si>
+    <t>Item 1</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Item 2</t>
+  </si>
+  <si>
+    <t>Item 3</t>
+  </si>
+  <si>
+    <t>Item 4</t>
+  </si>
+  <si>
+    <t>Cost</t>
   </si>
 </sst>
 </file>
@@ -357,167 +384,188 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{465E9103-4D3F-4595-974B-E0A7D6D30D40}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1001</v>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
       </c>
       <c r="B2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1001</v>
+        <v>11.5</v>
+      </c>
+      <c r="C2">
+        <v>6.125</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
       </c>
       <c r="B3">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>1001</v>
-      </c>
-      <c r="B4">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>1002</v>
-      </c>
-      <c r="B5">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>1002</v>
-      </c>
-      <c r="B6">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>1002</v>
-      </c>
-      <c r="B7">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>1003</v>
-      </c>
-      <c r="B8">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>1003</v>
-      </c>
-      <c r="B9">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4F4A73B-CB77-4221-A8FF-5D9604434D60}">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99FF2223-CC1A-4DC7-AE7C-5C9B40212755}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>11</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>22</v>
-      </c>
-      <c r="B3">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
+      <c r="E5">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>33</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>44</v>
-      </c>
-      <c r="B5">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5">
+      <c r="F5">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Worked on interpreting the test data
Almost complete with the function output. Should be able to use groupby and apply to pack each SO
</commit_message>
<xml_diff>
--- a/data_test.xlsx
+++ b/data_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mealt\Documents\GitHub\IE-431-Senior-Design-Telamon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422443EE-3255-4692-B986-2A5AB8A573B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BEE56FD-D48C-4599-B2D4-3ABE506370A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bins" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Length</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Bin 2</t>
   </si>
   <si>
-    <t>Item Name</t>
-  </si>
-  <si>
     <t>Item 1</t>
   </si>
   <si>
@@ -68,6 +65,12 @@
   </si>
   <si>
     <t>Cost</t>
+  </si>
+  <si>
+    <t>Sales Order Number</t>
+  </si>
+  <si>
+    <t>Item Number</t>
   </si>
 </sst>
 </file>
@@ -387,8 +390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{465E9103-4D3F-4595-974B-E0A7D6D30D40}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -410,7 +413,7 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -461,111 +464,126 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99FF2223-CC1A-4DC7-AE7C-5C9B40212755}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1001</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1001</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
         <v>8</v>
       </c>
-      <c r="B2">
+      <c r="E3">
         <v>5</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>8</v>
-      </c>
-      <c r="D3">
-        <v>5</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1002</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1002</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>12</v>
-      </c>
-      <c r="D4">
-        <v>7</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
       <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
         <v>6</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
       <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Code is messy but have a function that does pack shipping orders
</commit_message>
<xml_diff>
--- a/data_test.xlsx
+++ b/data_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mealt\Documents\GitHub\IE-431-Senior-Design-Telamon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BEE56FD-D48C-4599-B2D4-3ABE506370A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC58759-630D-41A0-9F78-6219169F40CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Length</t>
   </si>
@@ -71,6 +71,36 @@
   </si>
   <si>
     <t>Item Number</t>
+  </si>
+  <si>
+    <t>Unit Length</t>
+  </si>
+  <si>
+    <t>Unit Width</t>
+  </si>
+  <si>
+    <t>Unit Height</t>
+  </si>
+  <si>
+    <t>Unit Weight</t>
+  </si>
+  <si>
+    <t>20x20x30</t>
+  </si>
+  <si>
+    <t>11x11x5</t>
+  </si>
+  <si>
+    <t>22x22x18</t>
+  </si>
+  <si>
+    <t>16x16x16</t>
+  </si>
+  <si>
+    <t>24x24x24</t>
+  </si>
+  <si>
+    <t>26x15x7</t>
   </si>
 </sst>
 </file>
@@ -388,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{465E9103-4D3F-4595-974B-E0A7D6D30D40}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -454,6 +484,126 @@
       </c>
       <c r="F3">
         <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>30</v>
+      </c>
+      <c r="E4">
+        <v>50</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6">
+        <v>22</v>
+      </c>
+      <c r="C6">
+        <v>22</v>
+      </c>
+      <c r="D6">
+        <v>18</v>
+      </c>
+      <c r="E6">
+        <v>20</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>16</v>
+      </c>
+      <c r="D7">
+        <v>16</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8">
+        <v>24</v>
+      </c>
+      <c r="C8">
+        <v>24</v>
+      </c>
+      <c r="D8">
+        <v>24</v>
+      </c>
+      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9">
+        <v>26</v>
+      </c>
+      <c r="C9">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>20</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -467,7 +617,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -483,16 +633,16 @@
         <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="F1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="G1" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>